<commit_message>
Got logic for 2 player to work
</commit_message>
<xml_diff>
--- a/static/rhythm_games/No Overlap Fever.xlsx
+++ b/static/rhythm_games/No Overlap Fever.xlsx
@@ -604,7 +604,7 @@
         <v>13</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>19</v>
@@ -630,7 +630,7 @@
         <v>13</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6" s="9" t="s">
         <v>21</v>
@@ -656,7 +656,7 @@
         <v>13</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G7" s="9" t="s">
         <v>23</v>
@@ -682,7 +682,7 @@
         <v>13</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>25</v>
@@ -708,7 +708,7 @@
         <v>13</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G9" s="9" t="s">
         <v>27</v>
@@ -734,7 +734,7 @@
         <v>13</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>29</v>
@@ -760,7 +760,7 @@
         <v>13</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>31</v>
@@ -786,7 +786,7 @@
         <v>13</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>33</v>

</xml_diff>